<commit_message>
[siva]Add: Report generation for the FaceBook Automation
</commit_message>
<xml_diff>
--- a/Facebook_datatestdriven/Resources/Facebook_datadriventesting.xlsx
+++ b/Facebook_datatestdriven/Resources/Facebook_datadriventesting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\Facebook_datatestdriven\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\Facebook_datatestdriven\Facebook_datatestdriven\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880014BD-92E3-494D-A595-05358B22DF67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D882530-A2B6-4078-9A73-765A35266B3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{2711EC3A-45F8-43E9-A0BF-E846546FEE37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>login@123</t>
+    <t>Login@123</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[siva]Refactor: Refactoring code by  validation
</commit_message>
<xml_diff>
--- a/Facebook_datatestdriven/Resources/Facebook_datadriventesting.xlsx
+++ b/Facebook_datatestdriven/Resources/Facebook_datadriventesting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sivaranjani.b\source\repos\Facebook_datatestdriven\Facebook_datatestdriven\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D882530-A2B6-4078-9A73-765A35266B3C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D490F6-D687-48B6-9A87-D2A2192DE1B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{2711EC3A-45F8-43E9-A0BF-E846546FEE37}"/>
   </bookViews>
@@ -33,7 +33,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Login@123</t>
+    <t>siva123</t>
   </si>
 </sst>
 </file>
@@ -78,9 +78,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -417,8 +420,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>9786164316</v>
+      <c r="A2" s="2">
+        <v>8667361462</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -429,7 +432,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{38A961AA-553F-4501-9D58-8C081EEFC98B}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Login@123" xr:uid="{38A961AA-553F-4501-9D58-8C081EEFC98B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>